<commit_message>
include cost rate in sheet
</commit_message>
<xml_diff>
--- a/batt_sust_model/data/default_manufacturing_cost_parameters.xlsx
+++ b/batt_sust_model/data/default_manufacturing_cost_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joris\OneDrive - Newcastle University\Python\Projects\Batt_Sust_Model-1\batt_sust_model\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/b8061896_newcastle_ac_uk/Documents/Python/Projects/Batt_Sust_Model-1/batt_sust_model/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A8CD6D-A289-472A-8103-C94C88D4DE22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="13_ncr:1_{D9A8CD6D-A289-472A-8103-C94C88D4DE22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B479941-1724-479D-8ACA-A3B0DF367E86}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="volume_ratio_mapping" sheetId="4" r:id="rId5"/>
     <sheet name="volume_ratio_mapping_materials" sheetId="8" r:id="rId6"/>
     <sheet name="default_manufacturing_rates" sheetId="5" r:id="rId7"/>
-    <sheet name="process_mapping" sheetId="6" r:id="rId8"/>
+    <sheet name="cost_rates" sheetId="9" r:id="rId8"/>
+    <sheet name="process_mapping" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="114">
   <si>
     <t>cell stacking</t>
   </si>
@@ -326,6 +327,60 @@
   </si>
   <si>
     <t>material_exponent</t>
+  </si>
+  <si>
+    <t>variable_overhead_labor</t>
+  </si>
+  <si>
+    <t>pack_profit</t>
+  </si>
+  <si>
+    <t>working_capital</t>
+  </si>
+  <si>
+    <t>battery_warranty_costs</t>
+  </si>
+  <si>
+    <t>GSA_labour</t>
+  </si>
+  <si>
+    <t>r_and_d</t>
+  </si>
+  <si>
+    <t>launch_cost_labor</t>
+  </si>
+  <si>
+    <t>% annual variable cost</t>
+  </si>
+  <si>
+    <t>% of direct labor</t>
+  </si>
+  <si>
+    <t>% of investment</t>
+  </si>
+  <si>
+    <t>% of pack cost</t>
+  </si>
+  <si>
+    <t>% of depreciation</t>
+  </si>
+  <si>
+    <t>variable_overhead_depreciation</t>
+  </si>
+  <si>
+    <t>GSA_depreciation</t>
+  </si>
+  <si>
+    <t>lifetime_capital_equipment</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>launch_cost_material</t>
+  </si>
+  <si>
+    <t>% of direct material cost</t>
   </si>
 </sst>
 </file>
@@ -337,7 +392,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +427,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -402,13 +463,16 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{BBAD9B29-0260-4818-A730-1235CE0196AD}"/>
@@ -2065,8 +2129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A561B7B-0054-4D54-BE66-D844CA327308}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2240,6 +2304,170 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082350F5-846A-418F-B18C-1D27DF7D6F62}">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="6">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E004CA40-7BF9-4CA0-BA26-8A2A89620FCF}">
   <dimension ref="A1:B27"/>
   <sheetViews>

</xml_diff>